<commit_message>
funcionando retirada de capital
</commit_message>
<xml_diff>
--- a/JLP_2024-12.xlsx
+++ b/JLP_2024-12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,34 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Despesa</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Retirada de Capital</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>19/02/2025</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Luiz</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>